<commit_message>
SOECENT | fix Decade 2 footnotes jumplink and timeline item
</commit_message>
<xml_diff>
--- a/scripts/files/updated_timeline-prod.xlsx
+++ b/scripts/files/updated_timeline-prod.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccahong/programming/soe-centennial-nextjs/scripts/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F04E95-B257-D44A-B475-1536541E4FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E4E689-6D8F-4D4D-8105-864B7E692627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Timeline objects" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="611">
   <si>
     <t>year</t>
   </si>
@@ -2447,6 +2447,9 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/duv7bozlj/image/upload/v1745510375/20220301_Campus_N6A9748_kz2tmj.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/duv7bozlj/image/upload/v1742265422/SC0122_1998-144_b02_Computers_1985_0030_ma4z7u.jpg</t>
   </si>
 </sst>
 </file>
@@ -2535,6 +2538,7 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2855,8 +2859,8 @@
   <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E108" sqref="E108"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4244,7 +4248,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="56" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:5" ht="84" x14ac:dyDescent="0.15">
       <c r="A82" s="4">
         <v>1985</v>
       </c>
@@ -4257,8 +4261,8 @@
       <c r="D82" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="E82" s="10" t="s">
-        <v>325</v>
+      <c r="E82" s="18" t="s">
+        <v>610</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="84" x14ac:dyDescent="0.15">
@@ -5533,77 +5537,77 @@
     <hyperlink ref="E79" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
     <hyperlink ref="E80" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
     <hyperlink ref="E81" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="E82" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="E83" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="E84" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="E85" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="E86" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="E87" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="E88" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="E89" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="E90" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="E91" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="E92" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="E93" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="E94" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="E95" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="E96" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="E97" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="E98" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="E99" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="E100" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="E101" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="E102" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="E103" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="E104" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="E105" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="E106" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="E107" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="E109" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="E110" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="E111" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="E112" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="E113" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="E114" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="E115" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="E116" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="E117" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="E118" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="E119" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="E120" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="E121" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="E122" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="E123" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="E124" r:id="rId122" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="E125" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="E126" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="E127" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="E128" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="E129" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="E130" r:id="rId128" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="E131" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="E132" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="E133" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
-    <hyperlink ref="E134" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
-    <hyperlink ref="E135" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
-    <hyperlink ref="E136" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
-    <hyperlink ref="E137" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
-    <hyperlink ref="E138" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
-    <hyperlink ref="E139" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
-    <hyperlink ref="E140" r:id="rId138" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
-    <hyperlink ref="E141" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
-    <hyperlink ref="E142" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
-    <hyperlink ref="E143" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
-    <hyperlink ref="E144" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
-    <hyperlink ref="E145" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
-    <hyperlink ref="E146" r:id="rId144" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
-    <hyperlink ref="E147" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
-    <hyperlink ref="E148" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
-    <hyperlink ref="E149" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
-    <hyperlink ref="E150" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
-    <hyperlink ref="E151" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
-    <hyperlink ref="E152" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
-    <hyperlink ref="E108" r:id="rId151" xr:uid="{4939F33B-E536-CD41-9D50-47FF1305C38A}"/>
+    <hyperlink ref="E83" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="E84" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="E85" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="E86" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="E87" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="E88" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="E89" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="E90" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="E91" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="E92" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="E93" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="E94" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="E95" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="E96" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="E97" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="E98" r:id="rId96" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="E99" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="E100" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="E101" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="E102" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="E103" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="E104" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="E105" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="E106" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="E107" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="E109" r:id="rId106" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="E110" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="E111" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="E112" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="E113" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="E114" r:id="rId111" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="E115" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="E116" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="E117" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="E118" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="E119" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="E120" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="E121" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="E122" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="E123" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="E124" r:id="rId121" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="E125" r:id="rId122" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="E126" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="E127" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="E128" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="E129" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="E130" r:id="rId127" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="E131" r:id="rId128" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="E132" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="E133" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="E134" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="E135" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="E136" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="E137" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="E138" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="E139" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="E140" r:id="rId137" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="E141" r:id="rId138" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="E142" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="E143" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="E144" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="E145" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="E146" r:id="rId143" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="E147" r:id="rId144" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="E148" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="E149" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="E150" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="E151" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="E152" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="E108" r:id="rId150" xr:uid="{4939F33B-E536-CD41-9D50-47FF1305C38A}"/>
+    <hyperlink ref="E82" r:id="rId151" xr:uid="{B5A571B0-A2C4-8F4D-99EE-7E2095E917BA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>